<commit_message>
fix logger and add slap-audio
</commit_message>
<xml_diff>
--- a/study/Study_schedule.xlsx
+++ b/study/Study_schedule.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2459F4FF-6568-48AC-A8ED-2ADFC74B3C7B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-600" yWindow="4490" windowWidth="29430" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-600" yWindow="4485" windowWidth="29430" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -375,19 +374,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,7 +409,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -433,7 +432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -456,7 +455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -482,7 +481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -508,7 +507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -534,7 +533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -560,7 +559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -586,7 +585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -612,7 +611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -628,11 +627,14 @@
       <c r="E10">
         <v>3</v>
       </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
       <c r="G10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -655,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -678,7 +680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -701,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -724,7 +726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -747,7 +749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -770,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -793,7 +795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -816,7 +818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -839,7 +841,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -862,7 +864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -885,7 +887,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -908,7 +910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -931,7 +933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -954,7 +956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
changed schedule to latin square
</commit_message>
<xml_diff>
--- a/study/Study_schedule.xlsx
+++ b/study/Study_schedule.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380A6791-5282-42F4-B96A-BB793B9FEAB8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-600" yWindow="4485" windowWidth="29430" windowHeight="11820"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,11 +375,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,19 +418,19 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -437,22 +438,22 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -460,10 +461,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -472,10 +473,10 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K4" t="s">
         <v>12</v>
@@ -486,22 +487,22 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K5" t="s">
         <v>11</v>
@@ -512,22 +513,22 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K6" t="s">
         <v>10</v>
@@ -538,22 +539,22 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K7" t="s">
         <v>9</v>
@@ -564,22 +565,22 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <v>4</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K8" t="s">
         <v>8</v>
@@ -590,22 +591,22 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K9" t="s">
         <v>7</v>
@@ -616,22 +617,22 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -639,22 +640,22 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -662,22 +663,22 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -685,22 +686,22 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -711,19 +712,19 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -731,22 +732,22 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G15">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -754,22 +755,22 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -777,22 +778,22 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>5</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -800,22 +801,22 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G18">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -823,19 +824,19 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>6</v>
@@ -846,22 +847,22 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G20">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -872,19 +873,19 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G21">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -892,22 +893,22 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -915,22 +916,22 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F23">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -938,19 +939,19 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G24">
         <v>3</v>
@@ -961,22 +962,102 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>3</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>